<commit_message>
Final fase 2 estrategia
</commit_message>
<xml_diff>
--- a/docs/importantes/Acta de reunion ciclo 1.xlsx
+++ b/docs/importantes/Acta de reunion ciclo 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pryectos print(nul)\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e03e2c4a614451c2/Documentos/Bitacoras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77C6A46-E387-4BBC-885F-F085FB4A36B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{F829444C-2C9B-41BB-87A9-E68B081804F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8182FE5-8A31-4E49-A2EF-C0F6C8F149FE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{62DC227A-B2C0-4B2D-82A6-53B37F2213DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{62DC227A-B2C0-4B2D-82A6-53B37F2213DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Acta de Reuniones</t>
   </si>
@@ -87,16 +89,28 @@
   <si>
     <t>Se realizo la segunda reunion con el objetivo de coordinar y dejar todos los documentos
  relacionados a la primera entrega correctamente diligenciados</t>
+  </si>
+  <si>
+    <t>Se realizo la Tercera reunion con el objetivo de diligenciar el script de estrategias y repartir  
+los documentos correspondientes a administracion de configuraciones, plan de riesgos y definicion de estrategias</t>
+  </si>
+  <si>
+    <t>Documentacion Script de estrategias
+ y documentos relacionados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision documentos </t>
+  </si>
+  <si>
+    <t>Revision grupal de los documentos que se repartieron en la tercera reunion 
+(administracion de configuraciones, plan de riesgos y definicion de estrategias)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +197,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -193,9 +210,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -213,6 +227,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,52 +553,53 @@
   <dimension ref="B1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5" style="1"/>
-    <col min="3" max="3" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="92.375" style="1" customWidth="1"/>
-    <col min="8" max="12" width="11.5" style="1"/>
+    <col min="1" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.33203125" style="1" customWidth="1"/>
+    <col min="8" max="12" width="11.5546875" style="1"/>
     <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.5" style="1"/>
+    <col min="14" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="2:13">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="2:13" ht="15">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -618,97 +637,117 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="28.5">
+    <row r="4" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="4">
         <v>45877</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <v>0.5625</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="2:13" ht="28.5">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="4">
         <v>45880</v>
       </c>
-      <c r="D5" s="9">
-        <v>0.34027777777777779</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0.45833333333333331</v>
+      <c r="D5" s="5">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.90277777777777779</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="2:13">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="2:13">
+      <c r="C6" s="4">
+        <v>45889</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="2:13">
+      <c r="C7" s="4">
+        <v>45894</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>5</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -718,13 +757,13 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>

</xml_diff>